<commit_message>
added pydantic model validation
</commit_message>
<xml_diff>
--- a/app/excel.xlsx
+++ b/app/excel.xlsx
@@ -20,33 +20,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t xml:space="preserve">Item name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prompt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keywords</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Result</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+  <si>
+    <t xml:space="preserve">item_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prompt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keywords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">result</t>
   </si>
   <si>
     <t xml:space="preserve">Беспроводные наушники</t>
   </si>
   <si>
-    <t xml:space="preserve">Напиши мне описание беспроводных наушников от 4000 до 5000 символов. Важно не изменять ключевые слова и использовать их "как есть"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">наушники беспроводные, черные
-Наушники. Безпроводные,
-Наушники беспроводные большие черные,
-наушники черные,
-Беспроводные наушники черные,
-нушники беспроводные для телефона черные блютуз,
+    <t xml:space="preserve">Напиши мне описание беспроводных наушников от 4000 до 5000 символов. Важно не изменять ключевые слова и использовать их как есть</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Наушники беспроводные черные, Наушники Безпроводные,
+Наушники беспроводные большие черные, наушники черные, Беспроводные наушники черные, нушники беспроводные для телефона черные блютуз,
 гарнитур</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Беспроводные наушники 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Беспроводные наушники 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Беспроводные наушники 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Беспроводные наушники 5</t>
   </si>
 </sst>
 </file>
@@ -61,6 +69,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -120,12 +129,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -146,44 +159,88 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="38.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="180.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="79.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="79.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="79.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="79.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>